<commit_message>
added grading formula in results
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 101 Non CSE/results.xlsx
+++ b/FALL 19/CSE 101 Non CSE/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="quiz1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -185,13 +185,19 @@
   </si>
   <si>
     <t>Problem 4</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -222,6 +228,12 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +271,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,21 +494,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="6" width="14.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="2"/>
+    <col min="3" max="8" width="14.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +527,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>191011023</v>
       </c>
@@ -531,8 +554,16 @@
         <f t="shared" ref="F2:F49" si="0">C2+D2+E2</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="7">
+        <f>(F2/30)*100</f>
+        <v>100</v>
+      </c>
+      <c r="H2" s="8" t="str">
+        <f>IF(G2&gt;94,"A+",IF(G2&gt;84,"A",IF(G2&gt;79,"A-",IF(G2&gt;74,"B+",IF(G2&gt;69,"B",IF(G2&gt;64,"B-",IF(G2&gt;59,"C+",IF(G2&gt;54,"C",IF(G2&gt;49,"D","F")))))))))</f>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>191011053</v>
       </c>
@@ -552,8 +583,16 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G49" si="1">(F3/30)*100</f>
+        <v>90</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f t="shared" ref="H3:H49" si="2">IF(G3&gt;94,"A+",IF(G3&gt;84,"A",IF(G3&gt;79,"A-",IF(G3&gt;74,"B+",IF(G3&gt;69,"B",IF(G3&gt;64,"B-",IF(G3&gt;59,"C+",IF(G3&gt;54,"C",IF(G3&gt;49,"D","F")))))))))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>191011226</v>
       </c>
@@ -573,8 +612,16 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H4" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>192011003</v>
       </c>
@@ -588,8 +635,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>192011051</v>
       </c>
@@ -609,8 +664,16 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="9">
+        <f t="shared" si="1"/>
+        <v>63.333333333333329</v>
+      </c>
+      <c r="H6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>192011116</v>
       </c>
@@ -630,8 +693,16 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>192011156</v>
       </c>
@@ -651,8 +722,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>193011005</v>
       </c>
@@ -672,8 +751,16 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="9">
+        <f t="shared" si="1"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>193011025</v>
       </c>
@@ -693,8 +780,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>193011035</v>
       </c>
@@ -714,8 +809,16 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="9">
+        <f t="shared" si="1"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="H11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>193011069</v>
       </c>
@@ -735,8 +838,16 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>193011075</v>
       </c>
@@ -756,8 +867,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>193011105</v>
       </c>
@@ -775,8 +894,16 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="H14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>193011116</v>
       </c>
@@ -796,8 +923,16 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="H15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>193011117</v>
       </c>
@@ -817,8 +952,16 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="9">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>193011122</v>
       </c>
@@ -832,8 +975,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>193011123</v>
       </c>
@@ -853,8 +1004,16 @@
         <f t="shared" si="0"/>
         <v>26.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>88.333333333333329</v>
+      </c>
+      <c r="H18" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>193011128</v>
       </c>
@@ -868,8 +1027,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>193011133</v>
       </c>
@@ -889,8 +1056,16 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="9">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H20" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>193011152</v>
       </c>
@@ -910,8 +1085,16 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="H21" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>193011166</v>
       </c>
@@ -931,8 +1114,16 @@
         <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>81.666666666666671</v>
+      </c>
+      <c r="H22" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>193011176</v>
       </c>
@@ -952,8 +1143,16 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="7">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H23" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>193011181</v>
       </c>
@@ -973,8 +1172,16 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>36.666666666666664</v>
+      </c>
+      <c r="H24" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>193011185</v>
       </c>
@@ -994,8 +1201,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H25" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>193011189</v>
       </c>
@@ -1015,8 +1230,16 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="9">
+        <f t="shared" si="1"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="H26" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>193011194</v>
       </c>
@@ -1036,8 +1259,16 @@
         <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="9">
+        <f t="shared" si="1"/>
+        <v>91.666666666666657</v>
+      </c>
+      <c r="H27" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>191012011</v>
       </c>
@@ -1057,8 +1288,16 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="9">
+        <f t="shared" si="1"/>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="H28" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>191012060</v>
       </c>
@@ -1078,8 +1317,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H29" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>191012061</v>
       </c>
@@ -1099,8 +1346,16 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="9">
+        <f t="shared" si="1"/>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="H30" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>173013015</v>
       </c>
@@ -1120,8 +1375,16 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H31" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>182013026</v>
       </c>
@@ -1135,8 +1398,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>193013005</v>
       </c>
@@ -1156,8 +1427,16 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="H33" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>193013006</v>
       </c>
@@ -1177,8 +1456,16 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="9">
+        <f t="shared" si="1"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="H34" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>193013008</v>
       </c>
@@ -1198,8 +1485,16 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="9">
+        <f t="shared" si="1"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="H35" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>193013015</v>
       </c>
@@ -1219,8 +1514,16 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="9">
+        <f t="shared" si="1"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="H36" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>193013021</v>
       </c>
@@ -1240,8 +1543,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H37" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>193013030</v>
       </c>
@@ -1261,8 +1572,16 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="7">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H38" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>193013038</v>
       </c>
@@ -1282,8 +1601,16 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="7">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H39" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>193013043</v>
       </c>
@@ -1303,8 +1630,16 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H40" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>193013046</v>
       </c>
@@ -1324,8 +1659,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H41" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>193013050</v>
       </c>
@@ -1345,8 +1688,16 @@
         <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="9">
+        <f t="shared" si="1"/>
+        <v>71.666666666666671</v>
+      </c>
+      <c r="H42" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>193013055</v>
       </c>
@@ -1360,8 +1711,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>193013088</v>
       </c>
@@ -1381,8 +1740,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H44" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>193013096</v>
       </c>
@@ -1402,8 +1769,16 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="H45" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>182014039</v>
       </c>
@@ -1423,8 +1798,16 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G46" s="9">
+        <f t="shared" si="1"/>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="H46" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>183016004</v>
       </c>
@@ -1444,8 +1827,16 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="H47" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>193016002</v>
       </c>
@@ -1465,8 +1856,16 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H48" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>193016004</v>
       </c>
@@ -1485,6 +1884,14 @@
       <c r="F49" s="5">
         <f t="shared" si="0"/>
         <v>23.5</v>
+      </c>
+      <c r="G49" s="9">
+        <f t="shared" si="1"/>
+        <v>78.333333333333329</v>
+      </c>
+      <c r="H49" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B+</v>
       </c>
     </row>
   </sheetData>
@@ -1495,21 +1902,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="7" width="14.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="8" width="14.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,8 +1939,14 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>191011023</v>
       </c>
@@ -1551,8 +1965,16 @@
         <f>C2+D2+E2+F2</f>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="7">
+        <f>(G2/20)*100</f>
+        <v>22.5</v>
+      </c>
+      <c r="I2" s="8" t="str">
+        <f>IF(H2&gt;94,"A+",IF(H2&gt;84,"A",IF(H2&gt;79,"A-",IF(H2&gt;74,"B+",IF(H2&gt;69,"B",IF(H2&gt;64,"B-",IF(H2&gt;59,"C+",IF(H2&gt;54,"C",IF(H2&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>191011053</v>
       </c>
@@ -1575,8 +1997,16 @@
         <f t="shared" ref="G3:G49" si="0">C3+D3+E3+F3</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H49" si="1">(G3/20)*100</f>
+        <v>45</v>
+      </c>
+      <c r="I3" s="8" t="str">
+        <f t="shared" ref="I3:I49" si="2">IF(H3&gt;94,"A+",IF(H3&gt;84,"A",IF(H3&gt;79,"A-",IF(H3&gt;74,"B+",IF(H3&gt;69,"B",IF(H3&gt;64,"B-",IF(H3&gt;59,"C+",IF(H3&gt;54,"C",IF(H3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>191011226</v>
       </c>
@@ -1595,8 +2025,16 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I4" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>192011003</v>
       </c>
@@ -1611,8 +2049,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>192011051</v>
       </c>
@@ -1635,8 +2081,16 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>192011116</v>
       </c>
@@ -1659,8 +2113,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="I7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>192011156</v>
       </c>
@@ -1683,8 +2145,16 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="I8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>193011005</v>
       </c>
@@ -1703,8 +2173,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>193011025</v>
       </c>
@@ -1727,8 +2205,16 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>193011035</v>
       </c>
@@ -1751,8 +2237,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="I11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>193011069</v>
       </c>
@@ -1767,8 +2261,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>193011075</v>
       </c>
@@ -1789,8 +2291,16 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="7">
+        <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="I13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>193011105</v>
       </c>
@@ -1807,8 +2317,16 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="7">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="I14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>193011116</v>
       </c>
@@ -1829,8 +2347,16 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="7">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>193011117</v>
       </c>
@@ -1853,8 +2379,16 @@
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="7">
+        <f t="shared" si="1"/>
+        <v>62.5</v>
+      </c>
+      <c r="I16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>193011122</v>
       </c>
@@ -1869,8 +2403,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>193011123</v>
       </c>
@@ -1891,8 +2433,16 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="7">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I18" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>193011128</v>
       </c>
@@ -1915,8 +2465,16 @@
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="7">
+        <f t="shared" si="1"/>
+        <v>42.5</v>
+      </c>
+      <c r="I19" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>193011133</v>
       </c>
@@ -1939,8 +2497,16 @@
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="7">
+        <f t="shared" si="1"/>
+        <v>32.5</v>
+      </c>
+      <c r="I20" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>193011152</v>
       </c>
@@ -1961,8 +2527,16 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="7">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="I21" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>193011166</v>
       </c>
@@ -1985,8 +2559,16 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="7">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="I22" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>193011176</v>
       </c>
@@ -2007,8 +2589,16 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="7">
+        <f t="shared" si="1"/>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="I23" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>193011181</v>
       </c>
@@ -2029,8 +2619,16 @@
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="7">
+        <f t="shared" si="1"/>
+        <v>32.5</v>
+      </c>
+      <c r="I24" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>193011185</v>
       </c>
@@ -2051,8 +2649,16 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="7">
+        <f t="shared" si="1"/>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="I25" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>193011189</v>
       </c>
@@ -2075,8 +2681,16 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I26" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>193011194</v>
       </c>
@@ -2095,8 +2709,16 @@
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="7">
+        <f t="shared" si="1"/>
+        <v>27.500000000000004</v>
+      </c>
+      <c r="I27" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>191012011</v>
       </c>
@@ -2115,8 +2737,16 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="7">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I28" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>191012060</v>
       </c>
@@ -2139,8 +2769,16 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I29" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>191012061</v>
       </c>
@@ -2155,8 +2793,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>173013015</v>
       </c>
@@ -2179,8 +2825,16 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="I31" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>182013026</v>
       </c>
@@ -2199,8 +2853,16 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I32" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>193013005</v>
       </c>
@@ -2217,8 +2879,16 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I33" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>193013006</v>
       </c>
@@ -2241,8 +2911,16 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="7">
+        <f t="shared" si="1"/>
+        <v>47.5</v>
+      </c>
+      <c r="I34" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>193013008</v>
       </c>
@@ -2265,8 +2943,16 @@
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="7">
+        <f t="shared" si="1"/>
+        <v>67.5</v>
+      </c>
+      <c r="I35" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>193013015</v>
       </c>
@@ -2287,8 +2973,16 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="7">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I36" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>193013021</v>
       </c>
@@ -2311,8 +3005,16 @@
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="7">
+        <f t="shared" si="1"/>
+        <v>97.5</v>
+      </c>
+      <c r="I37" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>193013030</v>
       </c>
@@ -2335,8 +3037,16 @@
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="7">
+        <f t="shared" si="1"/>
+        <v>52.5</v>
+      </c>
+      <c r="I38" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>193013038</v>
       </c>
@@ -2357,8 +3067,16 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I39" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>193013043</v>
       </c>
@@ -2377,8 +3095,16 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I40" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>193013046</v>
       </c>
@@ -2393,8 +3119,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>193013050</v>
       </c>
@@ -2409,8 +3143,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>193013055</v>
       </c>
@@ -2433,8 +3175,16 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="7">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+      <c r="I43" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>193013088</v>
       </c>
@@ -2457,8 +3207,16 @@
         <f t="shared" si="0"/>
         <v>15.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="7">
+        <f t="shared" si="1"/>
+        <v>77.5</v>
+      </c>
+      <c r="I44" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>193013096</v>
       </c>
@@ -2481,8 +3239,16 @@
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="7">
+        <f t="shared" si="1"/>
+        <v>57.499999999999993</v>
+      </c>
+      <c r="I45" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>182014039</v>
       </c>
@@ -2501,8 +3267,16 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I46" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>183016004</v>
       </c>
@@ -2525,8 +3299,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="I47" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>193016002</v>
       </c>
@@ -2547,8 +3329,16 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="7">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+      <c r="I48" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>193016004</v>
       </c>
@@ -2569,8 +3359,17 @@
         <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
+      <c r="H49" s="7">
+        <f t="shared" si="1"/>
+        <v>72.5</v>
+      </c>
+      <c r="I49" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>